<commit_message>
color per aircraft size
</commit_message>
<xml_diff>
--- a/verification_scenarios.xlsx
+++ b/verification_scenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jasmi\OneDrive\Documenten\GitHub\OperationsMaarDanGoed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE009E9D-43A8-4DF8-AC1E-3FD2EF55642A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3573BDA2-7FBD-4C7D-BE15-2F4453E69985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="verification set-up" sheetId="3" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="72">
   <si>
     <t>volgorde</t>
   </si>
@@ -261,6 +261,9 @@
   </si>
   <si>
     <t xml:space="preserve">NOTE bij scenario 6: scenario zoals hier beschreven werkte niet (infeasible model), dus aantal pax per vlucht gelijk gemaakt. Uitkomst klopt dan wel, maar zou in theorie ook toevallig kunnen zijn. </t>
+  </si>
+  <si>
+    <t>08:50</t>
   </si>
 </sst>
 </file>
@@ -655,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E05A90A3-D917-43FD-898F-EFC0804CDF33}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -833,7 +836,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E3"/>
+      <selection activeCell="A2" sqref="A2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1006,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32BDF516-80AC-45C8-8F33-34C2FC4733CB}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -1457,7 +1460,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E3"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1631,7 +1634,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -1727,7 +1730,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E3"/>
+      <selection activeCell="A2" sqref="A2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1802,10 +1805,10 @@
         <v>44</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F3">
         <v>50</v>
@@ -1901,7 +1904,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="A2" sqref="A2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -1940,17 +1943,17 @@
         <v>43</v>
       </c>
       <c r="C2" s="2">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="D2" s="2">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="E2" s="2">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="F2" s="2">
         <f>AVERAGE(C2:E2)</f>
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>54</v>
@@ -2014,7 +2017,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:E3"/>
+      <selection activeCell="A2" sqref="A2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2301,7 +2304,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="A2" sqref="A2:I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2475,7 +2478,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="A2" sqref="A2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -2584,21 +2587,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007DADB0BCDAFDB944AD9BE180C9424584" ma:contentTypeVersion="4" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="4d59d5810ff29c424ee505008f679286">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="df9788b5-c688-4cdd-9c83-a42ed71d29d3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e6be581cbbc737cc40dca8023b150d41" ns2:_="">
     <xsd:import namespace="df9788b5-c688-4cdd-9c83-a42ed71d29d3"/>
@@ -2742,24 +2730,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2395047B-0C3C-42E1-9CEA-37016DDE6523}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E92744F9-C092-4052-AB16-B800C207589A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{102D3359-883E-468D-98B8-7E54C6DE7244}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2775,4 +2761,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E92744F9-C092-4052-AB16-B800C207589A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2395047B-0C3C-42E1-9CEA-37016DDE6523}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>